<commit_message>
Password encryption of pdf files base on the pdf names & respective passwords provided in the Database\dataFiles.xlsx
</commit_message>
<xml_diff>
--- a/Database/Datafile.xlsx
+++ b/Database/Datafile.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B31374-2036-4C82-B76D-0267C57921E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30CE2A6-B893-4047-AE6E-B99E1E60D89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="qrCode" sheetId="2" r:id="rId2"/>
+    <sheet name="passwordEncryption" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
   <si>
     <t>State</t>
   </si>
@@ -69,6 +80,78 @@
   </si>
   <si>
     <t>pattanayakpurna189@gmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Conduct</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>10-06-2021</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Purna Chandra Pattanaik</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Dak No</t>
+  </si>
+  <si>
+    <t>Dak Date</t>
+  </si>
+  <si>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Field credit Officer</t>
+  </si>
+  <si>
+    <t>2345</t>
+  </si>
+  <si>
+    <t>7209</t>
+  </si>
+  <si>
+    <t>22345</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>PDFName</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -100,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -123,15 +206,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -473,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,4 +872,270 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C620EB-9973-40A8-B77D-163EE526EC22}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>34543</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3">
+        <v>10200</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="5" t="str">
+        <f>$F$1&amp;"-"&amp;F2&amp;","&amp;$G$1&amp;"-"&amp;G2&amp;","&amp;$H$1&amp;"-"&amp;H2&amp;","&amp;$I$1&amp;"-"&amp;I2&amp;","&amp;$J$1&amp;"-"&amp;J2</f>
+        <v>Name-Umakanta Pattanaik,Employee ID-10200,From-10-06-2021,To-10-06-2021,Conduct-Good</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>23454</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3">
+        <v>11298</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="5" t="str">
+        <f>$F$1&amp;"-"&amp;F3&amp;","&amp;$G$1&amp;"-"&amp;G3&amp;","&amp;$H$1&amp;"-"&amp;H3&amp;","&amp;$I$1&amp;"-"&amp;I3&amp;","&amp;$J$1&amp;"-"&amp;J3</f>
+        <v>Name-Purna Chandra Pattanaik,Employee ID-11298,From-10-06-2021,To-10-06-2021,Conduct-Good</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{888D6BE6-3962-4F85-845A-9CD39F9812E4}">
+      <formula1>"Mr.,Ms."</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3492B4AA-3B61-4066-A17B-0FB3ABAF1C17}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>